<commit_message>
- added evaluation matrix
</commit_message>
<xml_diff>
--- a/comparation.xlsx
+++ b/comparation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,13 +9,108 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>CQM</t>
+  </si>
+  <si>
+    <t>IDE</t>
+  </si>
+  <si>
+    <t>Eclipse</t>
+  </si>
+  <si>
+    <t>Jenkins</t>
+  </si>
+  <si>
+    <t>Teamcity</t>
+  </si>
+  <si>
+    <t>SonarQube</t>
+  </si>
+  <si>
+    <t>1. Prepare analysis</t>
+  </si>
+  <si>
+    <t>Tool easy and intuitive to configure?</t>
+  </si>
+  <si>
+    <t>Possible to add external analyzers?</t>
+  </si>
+  <si>
+    <t>Possible to configure the analyzers?</t>
+  </si>
+  <si>
+    <t>Possible to view the rules?</t>
+  </si>
+  <si>
+    <t>Possible to choose, add, edit, delete rules?</t>
+  </si>
+  <si>
+    <t>2. Run analysis</t>
+  </si>
+  <si>
+    <t>Easy and intuitive to start the analysis?</t>
+  </si>
+  <si>
+    <t>Possible to following the analysis progress?</t>
+  </si>
+  <si>
+    <t>3. Evaluate analysis results</t>
+  </si>
+  <si>
+    <t>Issue overview with severity levels?</t>
+  </si>
+  <si>
+    <t>Issue trend/history?</t>
+  </si>
+  <si>
+    <t>Issue - source code mapping?</t>
+  </si>
+  <si>
+    <t>Issue description?</t>
+  </si>
+  <si>
+    <t>Issue description understandable?</t>
+  </si>
+  <si>
+    <t>Issue solution suggestion?</t>
+  </si>
+  <si>
+    <t>Issue filter options?</t>
+  </si>
+  <si>
+    <t>Edit issue status?</t>
+  </si>
+  <si>
+    <t>Delegate issues?</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>4. Manage  results</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,16 +118,57 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Marlett"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Marlett"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Marlett"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -40,18 +176,222 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +438,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +473,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +681,315 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="0.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="12"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
+    </row>
+    <row r="9" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="41">
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- added hamzas evaluation
</commit_message>
<xml_diff>
--- a/comparation.xlsx
+++ b/comparation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Questions</t>
   </si>
@@ -110,7 +110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +147,13 @@
       <name val="Marlett"/>
       <charset val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -299,22 +306,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -326,56 +321,104 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -685,7 +728,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,253 +743,312 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="28"/>
+      <c r="G1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="12"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12" t="s">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="12"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
+      <c r="F3" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
+      <c r="C4" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
+      <c r="C5" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="36"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
+      <c r="C6" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="36"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
+      <c r="C7" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="36"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20"/>
+      <c r="C8" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="40"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="28" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
+      <c r="C9" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="38"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="3"/>
+      <c r="C10" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="42"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="27"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
+      <c r="C11" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
+      <c r="C12" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23"/>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
+      <c r="C13" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
+      <c r="C14" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="36"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
     </row>
     <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
+      <c r="C15" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="36"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="23"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
+      <c r="C16" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="36"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="23"/>
     </row>
     <row r="17" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="20"/>
+      <c r="C17" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="21"/>
     </row>
     <row r="18" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="22" t="s">
+      <c r="A18" s="18"/>
+      <c r="B18" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="26"/>
+      <c r="C18" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="34"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G11:H11"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A16"/>
@@ -963,31 +1065,6 @@
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>